<commit_message>
Update importStudents, term, login controller and student model
</commit_message>
<xml_diff>
--- a/public/uploads/students.xlsx
+++ b/public/uploads/students.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document_University\DATN\data-import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326F795C-4667-420D-9E52-41F1DD7D15A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA2A06-3A35-439D-850A-774C64670461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF3A33CB-182B-40E2-BCA0-B0DD0080AFD3}"/>
   </bookViews>
@@ -1057,11 +1057,12 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="21.77734375" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" customWidth="1"/>

</xml_diff>

<commit_message>
Update all models and student, lecturer, groupStudent controllers
</commit_message>
<xml_diff>
--- a/public/uploads/students.xlsx
+++ b/public/uploads/students.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA2A06-3A35-439D-850A-774C64670461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D23C89-F558-4853-A5E4-2C52FE4085D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF3A33CB-182B-40E2-BCA0-B0DD0080AFD3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="191">
   <si>
     <t>STT</t>
   </si>
@@ -600,13 +600,22 @@
   </si>
   <si>
     <t>0972211749</t>
+  </si>
+  <si>
+    <t>30/04/2002</t>
+  </si>
+  <si>
+    <t>0972211750</t>
+  </si>
+  <si>
+    <t>DHKTPM15C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,6 +648,12 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1054,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B5DE1A-6501-43C8-AF7B-89255A320B4B}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2343,7 +2358,34 @@
         <v>18</v>
       </c>
     </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3">
+        <v>19525742</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update term, student, groupStudent controllers and termDetail model
</commit_message>
<xml_diff>
--- a/public/uploads/students.xlsx
+++ b/public/uploads/students.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D23C89-F558-4853-A5E4-2C52FE4085D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE059D9-B790-436C-A5B9-AE86B0FC128D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF3A33CB-182B-40E2-BCA0-B0DD0080AFD3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="144">
   <si>
     <t>STT</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Giới tính</t>
   </si>
   <si>
-    <t>Ngày sinh</t>
-  </si>
-  <si>
     <t>Số điện thoại</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Nam</t>
   </si>
   <si>
-    <t>04/01/2001</t>
-  </si>
-  <si>
     <t>0338618229</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>Đạt</t>
   </si>
   <si>
-    <t>17/05/2001</t>
-  </si>
-  <si>
     <t>0867490052</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>Phạm Thành</t>
   </si>
   <si>
-    <t>02/01/2001</t>
-  </si>
-  <si>
     <t>0339686430</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>Dự</t>
   </si>
   <si>
-    <t>16/02/2001</t>
-  </si>
-  <si>
     <t>0345136453</t>
   </si>
   <si>
@@ -122,18 +107,12 @@
     <t>Đức</t>
   </si>
   <si>
-    <t>12/05/2001</t>
-  </si>
-  <si>
     <t>0334548131</t>
   </si>
   <si>
     <t>Tăng Thanh</t>
   </si>
   <si>
-    <t>22/07/2001</t>
-  </si>
-  <si>
     <t>0983518610</t>
   </si>
   <si>
@@ -143,9 +122,6 @@
     <t>Duy</t>
   </si>
   <si>
-    <t>24/08/2001</t>
-  </si>
-  <si>
     <t>0793464997</t>
   </si>
   <si>
@@ -158,9 +134,6 @@
     <t>Nữ</t>
   </si>
   <si>
-    <t>10/02/2001</t>
-  </si>
-  <si>
     <t>0973087171</t>
   </si>
   <si>
@@ -170,9 +143,6 @@
     <t>Giang</t>
   </si>
   <si>
-    <t>14/09/2001</t>
-  </si>
-  <si>
     <t>0838607012</t>
   </si>
   <si>
@@ -188,18 +158,12 @@
     <t>Tô Đức</t>
   </si>
   <si>
-    <t>20/10/2001</t>
-  </si>
-  <si>
     <t>0372460109</t>
   </si>
   <si>
     <t>Trần Minh</t>
   </si>
   <si>
-    <t>24/09/2001</t>
-  </si>
-  <si>
     <t>0869648453</t>
   </si>
   <si>
@@ -209,9 +173,6 @@
     <t>Hòa</t>
   </si>
   <si>
-    <t>16/01/2001</t>
-  </si>
-  <si>
     <t>0356415806</t>
   </si>
   <si>
@@ -221,18 +182,12 @@
     <t>Hoàng</t>
   </si>
   <si>
-    <t>25/11/2001</t>
-  </si>
-  <si>
     <t>0973704198</t>
   </si>
   <si>
     <t>Vũ Huy</t>
   </si>
   <si>
-    <t>26/02/2001</t>
-  </si>
-  <si>
     <t>0917789964</t>
   </si>
   <si>
@@ -242,9 +197,6 @@
     <t>Hồng</t>
   </si>
   <si>
-    <t>16/12/2001</t>
-  </si>
-  <si>
     <t>0387267892</t>
   </si>
   <si>
@@ -254,9 +206,6 @@
     <t>Huân</t>
   </si>
   <si>
-    <t>02/10/2001</t>
-  </si>
-  <si>
     <t>0974822904</t>
   </si>
   <si>
@@ -266,36 +215,24 @@
     <t>Huy</t>
   </si>
   <si>
-    <t>10/06/2001</t>
-  </si>
-  <si>
     <t>0342409507</t>
   </si>
   <si>
     <t>Phạm Hoàng</t>
   </si>
   <si>
-    <t>18/01/2001</t>
-  </si>
-  <si>
     <t>0964505517</t>
   </si>
   <si>
     <t>Tống Gia</t>
   </si>
   <si>
-    <t>02/12/2001</t>
-  </si>
-  <si>
     <t>0902642161</t>
   </si>
   <si>
     <t>Vũ Quang</t>
   </si>
   <si>
-    <t>18/02/2001</t>
-  </si>
-  <si>
     <t>0984218514</t>
   </si>
   <si>
@@ -305,9 +242,6 @@
     <t>Kha</t>
   </si>
   <si>
-    <t>28/10/2001</t>
-  </si>
-  <si>
     <t>0833352650</t>
   </si>
   <si>
@@ -326,18 +260,12 @@
     <t>Lưu</t>
   </si>
   <si>
-    <t>07/02/2001</t>
-  </si>
-  <si>
     <t>0333751890</t>
   </si>
   <si>
     <t>Nguyễn Huy</t>
   </si>
   <si>
-    <t>26/01/2001</t>
-  </si>
-  <si>
     <t>0932669483</t>
   </si>
   <si>
@@ -347,9 +275,6 @@
     <t>Nghị</t>
   </si>
   <si>
-    <t>20/05/2001</t>
-  </si>
-  <si>
     <t>0378929240</t>
   </si>
   <si>
@@ -359,18 +284,12 @@
     <t>Nhân</t>
   </si>
   <si>
-    <t>01/05/2001</t>
-  </si>
-  <si>
     <t>0373523365</t>
   </si>
   <si>
     <t>Phát</t>
   </si>
   <si>
-    <t>10/01/2001</t>
-  </si>
-  <si>
     <t>0798522149</t>
   </si>
   <si>
@@ -380,9 +299,6 @@
     <t>Phong</t>
   </si>
   <si>
-    <t>15/11/2001</t>
-  </si>
-  <si>
     <t>0375559875</t>
   </si>
   <si>
@@ -392,9 +308,6 @@
     <t>Phú</t>
   </si>
   <si>
-    <t>26/07/2001</t>
-  </si>
-  <si>
     <t>0386267998</t>
   </si>
   <si>
@@ -404,9 +317,6 @@
     <t>Quân</t>
   </si>
   <si>
-    <t>02/08/2001</t>
-  </si>
-  <si>
     <t>0372253664</t>
   </si>
   <si>
@@ -416,27 +326,18 @@
     <t>Quang</t>
   </si>
   <si>
-    <t>02/09/2001</t>
-  </si>
-  <si>
     <t>0342455466</t>
   </si>
   <si>
     <t>Trần Vinh</t>
   </si>
   <si>
-    <t>13/07/2001</t>
-  </si>
-  <si>
     <t>0387383927</t>
   </si>
   <si>
     <t>Quý</t>
   </si>
   <si>
-    <t>11/09/2001</t>
-  </si>
-  <si>
     <t>0345634374</t>
   </si>
   <si>
@@ -446,9 +347,6 @@
     <t>Sáng</t>
   </si>
   <si>
-    <t>05/03/2001</t>
-  </si>
-  <si>
     <t>0346204298</t>
   </si>
   <si>
@@ -458,9 +356,6 @@
     <t>Sơn</t>
   </si>
   <si>
-    <t>26/04/2001</t>
-  </si>
-  <si>
     <t>0378390223</t>
   </si>
   <si>
@@ -470,9 +365,6 @@
     <t>Sỹ</t>
   </si>
   <si>
-    <t>22/05/2001</t>
-  </si>
-  <si>
     <t>0822159420</t>
   </si>
   <si>
@@ -482,9 +374,6 @@
     <t>Tài</t>
   </si>
   <si>
-    <t>24/03/2001</t>
-  </si>
-  <si>
     <t>0917482790</t>
   </si>
   <si>
@@ -494,9 +383,6 @@
     <t>Thuận</t>
   </si>
   <si>
-    <t>07/12/2001</t>
-  </si>
-  <si>
     <t>0817808173</t>
   </si>
   <si>
@@ -506,9 +392,6 @@
     <t>Thúy</t>
   </si>
   <si>
-    <t>05/05/2000</t>
-  </si>
-  <si>
     <t>0334838641</t>
   </si>
   <si>
@@ -521,9 +404,6 @@
     <t>Toàn</t>
   </si>
   <si>
-    <t>14/10/2001</t>
-  </si>
-  <si>
     <t>0867981145</t>
   </si>
   <si>
@@ -542,9 +422,6 @@
     <t>Trường</t>
   </si>
   <si>
-    <t>11/06/2000</t>
-  </si>
-  <si>
     <t>0378785836</t>
   </si>
   <si>
@@ -554,9 +431,6 @@
     <t>Văn</t>
   </si>
   <si>
-    <t>29/10/2001</t>
-  </si>
-  <si>
     <t>0963325802</t>
   </si>
   <si>
@@ -566,9 +440,6 @@
     <t>Việt</t>
   </si>
   <si>
-    <t>02/05/2001</t>
-  </si>
-  <si>
     <t>0983586953</t>
   </si>
   <si>
@@ -578,15 +449,9 @@
     <t>Vũ</t>
   </si>
   <si>
-    <t>24/05/2001</t>
-  </si>
-  <si>
     <t>0931866264</t>
   </si>
   <si>
-    <t>05/01/2001</t>
-  </si>
-  <si>
     <t>0919602469</t>
   </si>
   <si>
@@ -596,13 +461,7 @@
     <t>Vỹ</t>
   </si>
   <si>
-    <t>30/04/2001</t>
-  </si>
-  <si>
     <t>0972211749</t>
-  </si>
-  <si>
-    <t>30/04/2002</t>
   </si>
   <si>
     <t>0972211750</t>
@@ -1069,22 +928,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B5DE1A-6501-43C8-AF7B-89255A320B4B}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1106,11 +964,8 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1118,25 +973,22 @@
         <v>19470041</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1144,25 +996,22 @@
         <v>19439251</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1170,25 +1019,22 @@
         <v>19446101</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1196,25 +1042,22 @@
         <v>19509301</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1222,25 +1065,22 @@
         <v>19435491</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1248,25 +1088,22 @@
         <v>19475251</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1274,25 +1111,22 @@
         <v>19432121</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1300,25 +1134,22 @@
         <v>19469221</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1326,25 +1157,22 @@
         <v>19476751</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1352,25 +1180,22 @@
         <v>19522981</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1378,25 +1203,22 @@
         <v>19502521</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1404,25 +1226,22 @@
         <v>19434851</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1430,25 +1249,22 @@
         <v>19520101</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1456,25 +1272,22 @@
         <v>19508981</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1482,25 +1295,22 @@
         <v>19480271</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1508,25 +1318,22 @@
         <v>19524301</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1534,25 +1341,22 @@
         <v>19520901</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1560,25 +1364,22 @@
         <v>19481471</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1586,25 +1387,22 @@
         <v>19429061</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1612,25 +1410,22 @@
         <v>19470491</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1638,25 +1433,22 @@
         <v>19473311</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1664,25 +1456,22 @@
         <v>19431331</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1690,25 +1479,22 @@
         <v>19495701</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1716,25 +1502,22 @@
         <v>19482171</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1742,25 +1525,22 @@
         <v>19524231</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1768,25 +1548,22 @@
         <v>19495921</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1794,25 +1571,22 @@
         <v>19481331</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1820,25 +1594,22 @@
         <v>19483821</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1846,25 +1617,22 @@
         <v>19432841</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1872,25 +1640,22 @@
         <v>19476651</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1898,25 +1663,22 @@
         <v>19516911</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1924,25 +1686,22 @@
         <v>19495741</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1950,25 +1709,22 @@
         <v>19497751</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1976,25 +1732,22 @@
         <v>19485331</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2002,25 +1755,22 @@
         <v>19507801</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2028,25 +1778,22 @@
         <v>19508751</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2054,25 +1801,22 @@
         <v>19508311</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2080,25 +1824,22 @@
         <v>19498091</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2106,25 +1847,22 @@
         <v>19518101</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>151</v>
+        <v>114</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2132,25 +1870,22 @@
         <v>18062811</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2158,25 +1893,22 @@
         <v>19487901</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2184,25 +1916,22 @@
         <v>19486011</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2210,25 +1939,22 @@
         <v>19525251</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2236,25 +1962,22 @@
         <v>19503881</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2262,25 +1985,22 @@
         <v>19518901</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2288,25 +2008,22 @@
         <v>19501261</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2314,25 +2031,22 @@
         <v>19478651</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2340,25 +2054,22 @@
         <v>19525741</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2366,22 +2077,19 @@
         <v>19525742</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>190</v>
+        <v>142</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>